<commit_message>
ferramenta automatica incluida, estimativas
</commit_message>
<xml_diff>
--- a/FerramentaFPA-ProfRJP-Manual.xlsx
+++ b/FerramentaFPA-ProfRJP-Manual.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2TDSS\FerramentaFPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71173AA1-DCDD-413D-BF3D-679938A5DBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BD1F84-A8F4-4BA6-87F9-051D02556C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t>FERRAMENTA DE ESTIATIVA DE PONTOS DE SOFTWARE POR ANÁLISE DE PONTOS DE FUNÇÃO (FPA - FUNCTION POINT ANALYSIS)</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Frontend de manutançao de produto com recurso de consulta de produto</t>
   </si>
   <si>
-    <t>Arquivo de produto, Arquivo de exportação de produto</t>
-  </si>
-  <si>
     <t>Arquivo de historico de preço</t>
   </si>
   <si>
@@ -250,12 +247,49 @@
   <si>
     <t>Registro de produto</t>
   </si>
+  <si>
+    <t>idProd, cdProd, nmProd, vlProd, cdUnidMedida</t>
+  </si>
+  <si>
+    <t>idProd, dtInicioVigencia, dtFimVigencia, vlProd</t>
+  </si>
+  <si>
+    <t>idProd, cdProd, nmProd, vlProd, cdUnidMedida, dtExport</t>
+  </si>
+  <si>
+    <t>idProd, cdProd, nmProd, vlProd, cdUnidMedida, dtInicioVigencia, dtFimVigencia</t>
+  </si>
+  <si>
+    <t>idProd, vlProd, dtInicioVigencia, dtFimVigencia</t>
+  </si>
+  <si>
+    <t>cdProd, nmProd, vlProd, cdUnidMedida</t>
+  </si>
+  <si>
+    <t>idProd, cdProd, nmProd, vlProd, cdUnidMedida, vlNovoProd</t>
+  </si>
+  <si>
+    <t>IN:Arquivo de produto, 
+OUT: Arquivo de exportação de produto</t>
+  </si>
+  <si>
+    <t>IN: idProd, cdProd, nmProd, vlProd, cdUnidMedida
+OUT: idProd, cdProd, nmProd, vlProd, cdUnidMedida, dtExport</t>
+  </si>
+  <si>
+    <t>IN: 5
+OUT: 6</t>
+  </si>
+  <si>
+    <t>IN: 1
+OUT: 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +350,13 @@
       <b/>
       <sz val="14"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -614,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -683,6 +724,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1456,7 +1509,7 @@
   <dimension ref="A1:H240"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,7 +1592,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>54</v>
       </c>
@@ -1547,35 +1600,47 @@
         <v>7</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="31">
         <v>1</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
+      <c r="E9" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="31">
+        <v>5</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>22</v>
+      </c>
       <c r="H9" s="31"/>
     </row>
-    <row r="10" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="31">
         <v>1</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="34"/>
+      <c r="E10" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="31">
+        <v>4</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="31"/>
     </row>
-    <row r="11" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>55</v>
       </c>
@@ -1583,35 +1648,47 @@
         <v>8</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="31">
         <v>1</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="34"/>
+      <c r="E11" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="31">
+        <v>6</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="H11" s="31"/>
     </row>
-    <row r="12" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>56</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="31">
-        <v>2</v>
-      </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="34"/>
+      <c r="C12" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>22</v>
+      </c>
       <c r="H12" s="31"/>
     </row>
-    <row r="13" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>57</v>
       </c>
@@ -1619,14 +1696,20 @@
         <v>4</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="31">
         <v>2</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="34"/>
+      <c r="E13" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="31">
+        <v>7</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>20</v>
+      </c>
       <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1637,19 +1720,25 @@
         <v>4</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="31">
         <v>2</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="34"/>
+      <c r="E14" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="31">
+        <v>4</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="H14" s="31"/>
     </row>
     <row r="15" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>5</v>
@@ -1660,9 +1749,15 @@
       <c r="D15" s="31">
         <v>1</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="34"/>
+      <c r="E15" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="31">
+        <v>5</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="H15" s="31"/>
     </row>
     <row r="16" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1678,9 +1773,15 @@
       <c r="D16" s="31">
         <v>1</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="34"/>
+      <c r="E16" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="31">
+        <v>5</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1691,14 +1792,20 @@
         <v>4</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="31">
         <v>0</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="34"/>
+      <c r="E17" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="31">
+        <v>4</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1709,14 +1816,20 @@
         <v>4</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="31">
         <v>0</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="34"/>
+      <c r="E18" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="31">
+        <v>6</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1727,14 +1840,20 @@
         <v>5</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="31">
         <v>0</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="34"/>
+      <c r="E19" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="31">
+        <v>5</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="H19" s="31"/>
     </row>
     <row r="20" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>